<commit_message>
Add heroes to dr who videos
</commit_message>
<xml_diff>
--- a/Heroes.xlsx
+++ b/Heroes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="84" windowWidth="20100" windowHeight="5040"/>
+    <workbookView xWindow="96" yWindow="84" windowWidth="19416" windowHeight="5040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>Released</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -1156,6 +1153,9 @@
   </si>
   <si>
     <t>https://upload.wikimedia.org/wikipedia/en/thumb/0/0d/Samuel_power_at_full.jpg/375px-Samuel_power_at_full.jpg</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -1530,9 +1530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M79" sqref="M79"/>
+      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1560,42 +1560,42 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1607,21 +1607,21 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <f>F2+1</f>
@@ -1634,18 +1634,18 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F67" si="0">F3+1</f>
@@ -1658,18 +1658,18 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -1682,21 +1682,21 @@
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -1709,21 +1709,21 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -1736,21 +1736,21 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -1763,21 +1763,21 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -1790,21 +1790,21 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -1817,21 +1817,21 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -1844,21 +1844,21 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1871,26 +1871,26 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
       <c r="G13">
         <v>1</v>
       </c>
@@ -1898,21 +1898,21 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
@@ -1925,21 +1925,21 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -1952,21 +1952,21 @@
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1979,21 +1979,21 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -2006,21 +2006,21 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
@@ -2033,18 +2033,18 @@
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -2057,21 +2057,21 @@
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M19" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
@@ -2084,21 +2084,21 @@
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
@@ -2111,21 +2111,21 @@
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -2138,21 +2138,21 @@
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -2165,21 +2165,21 @@
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
@@ -2192,21 +2192,21 @@
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2218,21 +2218,21 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
@@ -2245,21 +2245,21 @@
         <v>1</v>
       </c>
       <c r="L26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
@@ -2272,21 +2272,21 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
@@ -2299,21 +2299,21 @@
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -2326,21 +2326,21 @@
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
@@ -2353,21 +2353,21 @@
         <v>1</v>
       </c>
       <c r="L30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
@@ -2380,21 +2380,21 @@
         <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
@@ -2407,21 +2407,21 @@
         <v>1</v>
       </c>
       <c r="L32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
@@ -2434,21 +2434,21 @@
         <v>1</v>
       </c>
       <c r="L33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
@@ -2461,21 +2461,21 @@
         <v>1</v>
       </c>
       <c r="L34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
@@ -2488,21 +2488,21 @@
         <v>1</v>
       </c>
       <c r="L35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M35" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2514,21 +2514,21 @@
         <v>1</v>
       </c>
       <c r="L36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
@@ -2541,21 +2541,21 @@
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M37" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
@@ -2568,21 +2568,21 @@
         <v>1</v>
       </c>
       <c r="L38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M38" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
@@ -2595,21 +2595,21 @@
         <v>1</v>
       </c>
       <c r="L39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
@@ -2622,21 +2622,21 @@
         <v>1</v>
       </c>
       <c r="L40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M40" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
@@ -2649,21 +2649,21 @@
         <v>1</v>
       </c>
       <c r="L41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
@@ -2676,21 +2676,21 @@
         <v>1</v>
       </c>
       <c r="L42" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M42" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
@@ -2703,21 +2703,21 @@
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M43" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
@@ -2730,21 +2730,21 @@
         <v>1</v>
       </c>
       <c r="L44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
@@ -2757,21 +2757,21 @@
         <v>1</v>
       </c>
       <c r="L45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M45" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
@@ -2784,21 +2784,21 @@
         <v>1</v>
       </c>
       <c r="L46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M46" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
@@ -2811,21 +2811,21 @@
         <v>1</v>
       </c>
       <c r="L47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M47" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
@@ -2838,21 +2838,21 @@
         <v>1</v>
       </c>
       <c r="L48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
@@ -2865,21 +2865,21 @@
         <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M49" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
@@ -2892,21 +2892,21 @@
         <v>1</v>
       </c>
       <c r="L50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M50" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
@@ -2919,21 +2919,21 @@
         <v>1</v>
       </c>
       <c r="L51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
@@ -2946,21 +2946,21 @@
         <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M52" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
@@ -2973,21 +2973,21 @@
         <v>1</v>
       </c>
       <c r="L53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
@@ -3000,21 +3000,21 @@
         <v>1</v>
       </c>
       <c r="L54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
@@ -3027,21 +3027,21 @@
         <v>1</v>
       </c>
       <c r="L55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M55" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
@@ -3054,21 +3054,21 @@
         <v>1</v>
       </c>
       <c r="L56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M56" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
@@ -3081,18 +3081,18 @@
         <v>1</v>
       </c>
       <c r="L57" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M57" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E58" s="6">
         <v>1961</v>
@@ -3108,21 +3108,21 @@
         <v>1</v>
       </c>
       <c r="L58" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
@@ -3135,21 +3135,21 @@
         <v>1</v>
       </c>
       <c r="L59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M59" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
@@ -3162,21 +3162,21 @@
         <v>1</v>
       </c>
       <c r="L60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M60" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E61" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -3188,21 +3188,21 @@
         <v>1</v>
       </c>
       <c r="L61" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M61" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E62" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
@@ -3215,21 +3215,21 @@
         <v>1</v>
       </c>
       <c r="L62" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M62" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
@@ -3242,21 +3242,21 @@
         <v>1</v>
       </c>
       <c r="L63" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M63" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
@@ -3269,21 +3269,21 @@
         <v>1</v>
       </c>
       <c r="L64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M64" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E65" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
@@ -3296,21 +3296,21 @@
         <v>1</v>
       </c>
       <c r="L65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M65" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E66" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F66">
         <f t="shared" si="0"/>
@@ -3323,21 +3323,21 @@
         <v>1</v>
       </c>
       <c r="L66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M66" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E67" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F67">
         <f t="shared" si="0"/>
@@ -3350,21 +3350,21 @@
         <v>1</v>
       </c>
       <c r="L67" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M67" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F68">
         <f t="shared" ref="F68:F78" si="1">F67+1</f>
@@ -3377,21 +3377,21 @@
         <v>1</v>
       </c>
       <c r="L68" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M68" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E69" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F69">
         <f t="shared" si="1"/>
@@ -3404,21 +3404,21 @@
         <v>1</v>
       </c>
       <c r="L69" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M69" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F70">
         <f t="shared" si="1"/>
@@ -3431,21 +3431,21 @@
         <v>1</v>
       </c>
       <c r="L70" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M70" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E71" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F71">
         <f t="shared" si="1"/>
@@ -3458,21 +3458,21 @@
         <v>1</v>
       </c>
       <c r="L71" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M71" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E72" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F72">
         <f t="shared" si="1"/>
@@ -3485,21 +3485,21 @@
         <v>1</v>
       </c>
       <c r="L72" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M72" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F73">
         <f t="shared" si="1"/>
@@ -3512,21 +3512,21 @@
         <v>1</v>
       </c>
       <c r="L73" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M73" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E74" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F74">
         <f t="shared" si="1"/>
@@ -3539,21 +3539,21 @@
         <v>1</v>
       </c>
       <c r="L74" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M74" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E75" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F75">
         <f t="shared" si="1"/>
@@ -3566,21 +3566,21 @@
         <v>1</v>
       </c>
       <c r="L75" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M75" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E76" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F76">
         <f t="shared" si="1"/>
@@ -3593,21 +3593,21 @@
         <v>1</v>
       </c>
       <c r="L76" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M76" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D77" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F77">
         <f t="shared" si="1"/>
@@ -3620,21 +3620,21 @@
         <v>1</v>
       </c>
       <c r="L77" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M77" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D78" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E78" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F78">
         <f t="shared" si="1"/>
@@ -3647,10 +3647,10 @@
         <v>1</v>
       </c>
       <c r="L78" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="M78" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -3679,19 +3679,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3702,19 +3702,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3725,19 +3725,19 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3748,19 +3748,19 @@
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3771,19 +3771,19 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -3794,19 +3794,19 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -3817,19 +3817,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3840,19 +3840,19 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -3863,19 +3863,19 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3886,19 +3886,19 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3909,19 +3909,19 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3932,19 +3932,19 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" t="s">
         <v>211</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" t="s">
         <v>212</v>
       </c>
-      <c r="E12" t="s">
-        <v>188</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>213</v>
-      </c>
-      <c r="G12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3955,19 +3955,19 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
         <v>215</v>
       </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" t="s">
         <v>216</v>
-      </c>
-      <c r="F13" t="s">
-        <v>213</v>
-      </c>
-      <c r="G13" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3978,19 +3978,19 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
         <v>218</v>
       </c>
-      <c r="D14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>219</v>
-      </c>
-      <c r="G14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -4001,19 +4001,19 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" t="s">
         <v>221</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" t="s">
         <v>222</v>
       </c>
-      <c r="E15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>223</v>
-      </c>
-      <c r="G15" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -4024,19 +4024,19 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" t="s">
         <v>225</v>
       </c>
-      <c r="D16" t="s">
-        <v>180</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>226</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>227</v>
-      </c>
-      <c r="G16" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -4047,19 +4047,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
         <v>229</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>230</v>
-      </c>
-      <c r="G17" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -4070,19 +4070,19 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
         <v>232</v>
       </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>233</v>
-      </c>
-      <c r="G18" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>